<commit_message>
fix link to template
</commit_message>
<xml_diff>
--- a/pkgdown/assets/metadata_mmu_template.xlsx
+++ b/pkgdown/assets/metadata_mmu_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domeally/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D969CCE4-3BD9-7C40-9F6D-A81678FB2F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C424C5-3CBE-834D-8C5F-53CF61281389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35520" yWindow="-2340" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="-35520" yWindow="-2340" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_mmu" sheetId="1" r:id="rId1"/>
-    <sheet name="Data validation" sheetId="2" r:id="rId2"/>
+    <sheet name="Data validation" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={8D776C04-5295-9B44-9A2C-956D587A55FC}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,11 +152,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,12 +290,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="37">
@@ -688,9 +682,9 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="16" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1059,11 +1053,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,19 +1222,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Data validation'!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Data validation'!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Data validation'!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -1253,10 +1247,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>